<commit_message>
Initial draft of responsibility matrix complete
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECEUWO\Teaching\Fall2017\SE3352A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leozhang/Git/Ademidun-Hart-Co/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -44,74 +50,128 @@
     <t>P: Primary   S: Support</t>
   </si>
   <si>
-    <t>Team Member 2</t>
-  </si>
-  <si>
-    <t>Team Member 3</t>
-  </si>
-  <si>
-    <t>Team Member 4</t>
-  </si>
-  <si>
-    <t>Team Member 5</t>
-  </si>
-  <si>
-    <t>Team Member 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Team Name: </t>
   </si>
   <si>
     <t>Project Name:</t>
   </si>
   <si>
-    <t>&lt;Add rows as necessary&gt;</t>
-  </si>
-  <si>
     <t>&lt;Enter task name, section number, or sib section number as it appears in the SRS template breakdown here&gt;</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Example)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SRS - Section 3.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Team Member 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Replace it by the correct team member name</t>
-    </r>
+    <t>Brian He</t>
+  </si>
+  <si>
+    <t>Sooruj Ghangass</t>
+  </si>
+  <si>
+    <t>Andrew Hart</t>
+  </si>
+  <si>
+    <t>Nicholas Vukelic</t>
+  </si>
+  <si>
+    <t>Tomiwa Ademidun</t>
+  </si>
+  <si>
+    <t>Ademidun Hart &amp; Co.</t>
+  </si>
+  <si>
+    <t>"Self Start" for Marcotte Physiotherapy</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.1 - Purpose</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.2 - Scope</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.3 - Definitions, Acronyms, and Abbreviations</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.4 - References</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.5 - Overview</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.1 Introduction</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.2 Survey Description</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.3 Use-Case Model Hierarchy</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.4 Diagrams of the Use-Case Model</t>
+  </si>
+  <si>
+    <t>Leo Zhang</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.2 Functional Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.3 Usability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.4 Reliability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.5 Performance</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.6 Supportability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.7 Design Constraints</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.8 Online User Documentation &amp; Help System Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.9 Purchased Components</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.1 User Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.2 Hardware Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.3 Software Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.4 Communication Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.11 Licensing Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.12 Legal, Copyright and Other Notices</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 1-6</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 13-18</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 7-12</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.13 Applicable Standards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,13 +198,6 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,28 +217,28 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -193,10 +246,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -205,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,33 +594,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="47.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,8 +636,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -583,30 +645,30 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -619,117 +681,473 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>25</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>26</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>27</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added updated files that included prior assigned tasks
</commit_message>
<xml_diff>
--- a/Responsibility Matrix.xlsx
+++ b/Responsibility Matrix.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ECEUWO\Teaching\Fall2017\SE3352A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leozhang/Git/Ademidun-Hart-Co/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13920" windowHeight="7200"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
   <si>
     <t>Responsibility Matrix</t>
   </si>
@@ -44,74 +50,128 @@
     <t>P: Primary   S: Support</t>
   </si>
   <si>
-    <t>Team Member 2</t>
-  </si>
-  <si>
-    <t>Team Member 3</t>
-  </si>
-  <si>
-    <t>Team Member 4</t>
-  </si>
-  <si>
-    <t>Team Member 5</t>
-  </si>
-  <si>
-    <t>Team Member 6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Team Name: </t>
   </si>
   <si>
     <t>Project Name:</t>
   </si>
   <si>
-    <t>&lt;Add rows as necessary&gt;</t>
-  </si>
-  <si>
     <t>&lt;Enter task name, section number, or sib section number as it appears in the SRS template breakdown here&gt;</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>(Example)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> SRS - Section 3.2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Team Member 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Replace it by the correct team member name</t>
-    </r>
+    <t>Brian He</t>
+  </si>
+  <si>
+    <t>Sooruj Ghangass</t>
+  </si>
+  <si>
+    <t>Andrew Hart</t>
+  </si>
+  <si>
+    <t>Nicholas Vukelic</t>
+  </si>
+  <si>
+    <t>Tomiwa Ademidun</t>
+  </si>
+  <si>
+    <t>Ademidun Hart &amp; Co.</t>
+  </si>
+  <si>
+    <t>"Self Start" for Marcotte Physiotherapy</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.1 - Purpose</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.2 - Scope</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.3 - Definitions, Acronyms, and Abbreviations</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.4 - References</t>
+  </si>
+  <si>
+    <t>SRS - Section 1.5 - Overview</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.1 Introduction</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.2 Survey Description</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.3 Use-Case Model Hierarchy</t>
+  </si>
+  <si>
+    <t>SRS - Section 2.1.4 Diagrams of the Use-Case Model</t>
+  </si>
+  <si>
+    <t>Leo Zhang</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.2 Functional Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.3 Usability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.4 Reliability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.5 Performance</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.6 Supportability</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.7 Design Constraints</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.8 Online User Documentation &amp; Help System Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.9 Purchased Components</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.1 User Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.2 Hardware Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.3 Software Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.10.4 Communication Interfaces</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.11 Licensing Requirements</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.12 Legal, Copyright and Other Notices</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 1-6</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 13-18</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.1 Use-Case 7-12</t>
+  </si>
+  <si>
+    <t>SRS - Section 3.13 Applicable Standards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,13 +198,6 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,28 +217,28 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -193,10 +246,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -205,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,33 +594,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="47.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -574,8 +636,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -583,30 +645,30 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="49.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>4</v>
@@ -619,117 +681,473 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>19</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>23</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>25</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>26</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>27</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>